<commit_message>
modfication to GA and preprocessing for EQ mod
</commit_message>
<xml_diff>
--- a/reg_file.xlsx
+++ b/reg_file.xlsx
@@ -413,22 +413,22 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>37.271943414119292</v>
+        <v>65.945913649036683</v>
       </c>
       <c r="D2">
-        <v>4.9095509828703108</v>
+        <v>0.86533237141068364</v>
       </c>
       <c r="E2">
-        <v>64.880786496026062</v>
+        <v>66.843945765149201</v>
       </c>
       <c r="F2">
-        <v>3.6394089481895593</v>
+        <v>0.97375581202086281</v>
       </c>
       <c r="G2">
-        <v>13.059132289218503</v>
+        <v>15.731999831838332</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -439,19 +439,19 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>69.138595681986729</v>
+        <v>60.281550895109795</v>
       </c>
       <c r="D3">
-        <v>3.4436475832912428</v>
+        <v>0.93453264185714435</v>
       </c>
       <c r="E3">
-        <v>60.677321095833989</v>
+        <v>49.272854016130395</v>
       </c>
       <c r="F3">
-        <v>3.8510576177926712</v>
+        <v>1.2044502233804624</v>
       </c>
       <c r="G3">
-        <v>15.288095816642763</v>
+        <v>20.664665002975042</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -459,22 +459,22 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>27.026732613120252</v>
+        <v>24.741887516206372</v>
       </c>
       <c r="D4">
-        <v>5.2953266347903449</v>
+        <v>1.2863969302859308</v>
       </c>
       <c r="E4">
-        <v>60.346352707826753</v>
+        <v>35.177898398257199</v>
       </c>
       <c r="F4">
-        <v>3.867230315703309</v>
+        <v>1.3615393447435347</v>
       </c>
       <c r="G4">
-        <v>14.55417068384221</v>
+        <v>21.631647537449201</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -482,22 +482,22 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>5779</v>
+        <v>1939</v>
       </c>
       <c r="C5">
-        <v>63.459042235259865</v>
+        <v>75.879453113362416</v>
       </c>
       <c r="D5">
-        <v>3.7471477800820128</v>
+        <v>0.72826914334596071</v>
       </c>
       <c r="E5">
-        <v>61.309951011545238</v>
+        <v>54.544833959881636</v>
       </c>
       <c r="F5">
-        <v>3.8263400856389627</v>
+        <v>1.1675916874235441</v>
       </c>
       <c r="G5">
-        <v>15.440812602126202</v>
+        <v>20.385222085635686</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -505,22 +505,22 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C6">
-        <v>69.167260561292693</v>
+        <v>82.034676572744075</v>
       </c>
       <c r="D6">
-        <v>3.4420479367960124</v>
+        <v>0.62851530004341649</v>
       </c>
       <c r="E6">
-        <v>66.351144060212746</v>
+        <v>60.509269546238301</v>
       </c>
       <c r="F6">
-        <v>3.5624076873971982</v>
+        <v>1.0627135685394753</v>
       </c>
       <c r="G6">
-        <v>13.851493540457643</v>
+        <v>17.355022868323601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>